<commit_message>
Refactored dropdown comp generation and added chart comp generation code
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6551189-8156-435C-B0C4-E36853E90811}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="59">
   <si>
     <t>Components</t>
   </si>
@@ -181,13 +175,34 @@
   </si>
   <si>
     <t>Languages</t>
+  </si>
+  <si>
+    <t>Chart</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Bar</t>
+  </si>
+  <si>
+    <t>Renewed Policies</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>{"maintainAspectRatio": false, "scales":{"yAxes":[{"ticks":{"beginAtZero":true}}]}}</t>
+  </si>
+  <si>
+    <t>{"labels":["January", "February", "March", "April", "May", "June"],"datasets":[{"label":"# of Policies Renewed","data":[12,19,3,5,2,3],"backgroundColor":["rgba(255, 99, 132, 0.2)","rgba(54, 162, 235, 0.2)","rgba(255, 206, 86, 0.2)","rgba(75, 192, 192, 0.2)","rgba(153, 102, 255, 0.2)","rgba(255, 159, 64, 0.2)"],"borderColor":["rgba(255, 99, 132, 1)","rgba(54, 162, 235, 1)","rgba(255, 206, 86, 1)","rgba(75, 192, 192, 1)","rgba(153, 102, 255, 1)","rgba(255, 159, 64, 1)"],"borderWidth":1}]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,8 +231,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,7 +294,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,7 +329,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -490,21 +506,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -517,7 +533,7 @@
     <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +583,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -575,7 +591,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -604,7 +620,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -639,7 +655,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -671,7 +687,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -706,7 +722,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -741,7 +757,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -782,7 +798,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -812,6 +828,35 @@
       </c>
       <c r="K9" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved the mandatory attribute
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B2BC10-C91C-4A45-9AAF-A928975259EE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -201,8 +207,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,21 +512,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -530,10 +536,10 @@
     <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +589,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -591,7 +597,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -620,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -655,7 +661,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -687,7 +693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -722,7 +728,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>30</v>
       </c>
@@ -757,7 +763,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -798,7 +804,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -830,7 +836,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
Fixing table field issue
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>Components</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>stickyHeader</t>
+  </si>
+  <si>
+    <t>Pie</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,6 +954,35 @@
         <v>1</v>
       </c>
     </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Addition of date picker
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E36006-475E-4396-8202-8EF59114AED0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Components</t>
   </si>
@@ -226,13 +232,28 @@
   </si>
   <si>
     <t>Pie</t>
+  </si>
+  <si>
+    <t>DatePicker</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>MM/dd/yyyy</t>
+  </si>
+  <si>
+    <t>Date of Birth:</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,21 +557,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -564,7 +585,7 @@
     <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +635,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -622,7 +643,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -651,7 +672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -686,7 +707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -721,7 +742,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -753,7 +774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -788,7 +809,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -823,7 +844,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -864,7 +885,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -896,7 +917,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -925,7 +946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -954,7 +975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -981,6 +1002,35 @@
       </c>
       <c r="J13" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added table component with api
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vscode-workspace\accenture\react-magneto-v1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B172122-A488-452C-B42A-1DDE729A8FA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="20736" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="67">
   <si>
     <t>Components</t>
   </si>
@@ -210,29 +216,23 @@
     <t>employeeTable</t>
   </si>
   <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>rows</t>
-  </si>
-  <si>
-    <t>[{ "field": "id", "label": "ID" }, { "field": "firstName", "label": "First name" }, { "field": "lastName", "label": "Last name" }, { "field": "age", "label": "Age", "type": "number" }]</t>
-  </si>
-  <si>
-    <t>[{ "id": 1, "lastName": "Snow", "firstName": "Jon", "age": 35 }, { "id": 2, "lastName": "Lannister", "firstName": "Cersei", "age": 42 }, { "id": 3, "lastName": "Lannister", "firstName": "Jaime", "age": 45 }, { "id": 4, "lastName": "Stark", "firstName": "Arya", "age": 16 }, { "id": 5, "lastName": "Targaryen", "firstName": "Daenerys", "age": 30 }, { "id": 6, "lastName": "Melisandre", "firstName": null, "age": 50 }, { "id": 7, "lastName": "Clifford", "firstName": "Ferrara", "age": 44 }, { "id": 8, "lastName": "Frances", "firstName": "Rossini", "age": 36 }, { "id": 9, "lastName": "Roxie", "firstName": "Harvey", "age": 65 }]</t>
-  </si>
-  <si>
     <t>stickyHeader</t>
   </si>
   <si>
     <t>Pie</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>http://localhost:9001/tableData</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,35 +536,35 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="75.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="75.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -614,7 +614,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -622,7 +622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -651,7 +651,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -686,7 +686,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -721,7 +721,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -753,7 +753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -788,7 +788,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -823,7 +823,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -864,7 +864,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -896,7 +896,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -925,7 +925,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -936,25 +936,19 @@
         <v>62</v>
       </c>
       <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" t="b">
+      <c r="H12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -962,7 +956,7 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -985,5 +979,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding Search Field component
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -1,23 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lohith_R\Documents\LatestCode\react-magneto-v1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E36006-475E-4396-8202-8EF59114AED0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
   <si>
     <t>Components</t>
   </si>
@@ -247,13 +241,28 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t>SearchField</t>
+  </si>
+  <si>
+    <t>sicCode</t>
+  </si>
+  <si>
+    <t>SIC Code</t>
+  </si>
+  <si>
+    <t>SIC Code:</t>
+  </si>
+  <si>
+    <t>placeHolder</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -557,21 +566,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
@@ -585,7 +594,7 @@
     <col min="12" max="12" width="75.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -635,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -643,7 +652,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -672,7 +681,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -707,7 +716,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -742,7 +751,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -774,7 +783,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -809,7 +818,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -844,7 +853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -885,7 +894,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -917,7 +926,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>52</v>
       </c>
@@ -946,7 +955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -975,7 +984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>52</v>
       </c>
@@ -1004,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -1031,6 +1040,35 @@
       </c>
       <c r="J14" s="1" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting table data from API(Rohan changes)
</commit_message>
<xml_diff>
--- a/ui1.xlsx
+++ b/ui1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="77">
   <si>
     <t>Components</t>
   </si>
@@ -210,18 +210,6 @@
     <t>employeeTable</t>
   </si>
   <si>
-    <t>columns</t>
-  </si>
-  <si>
-    <t>rows</t>
-  </si>
-  <si>
-    <t>[{ "field": "id", "label": "ID" }, { "field": "firstName", "label": "First name" }, { "field": "lastName", "label": "Last name" }, { "field": "age", "label": "Age", "type": "number" }]</t>
-  </si>
-  <si>
-    <t>[{ "id": 1, "lastName": "Snow", "firstName": "Jon", "age": 35 }, { "id": 2, "lastName": "Lannister", "firstName": "Cersei", "age": 42 }, { "id": 3, "lastName": "Lannister", "firstName": "Jaime", "age": 45 }, { "id": 4, "lastName": "Stark", "firstName": "Arya", "age": 16 }, { "id": 5, "lastName": "Targaryen", "firstName": "Daenerys", "age": 30 }, { "id": 6, "lastName": "Melisandre", "firstName": null, "age": 50 }, { "id": 7, "lastName": "Clifford", "firstName": "Ferrara", "age": 44 }, { "id": 8, "lastName": "Frances", "firstName": "Rossini", "age": 36 }, { "id": 9, "lastName": "Roxie", "firstName": "Harvey", "age": 65 }]</t>
-  </si>
-  <si>
     <t>stickyHeader</t>
   </si>
   <si>
@@ -256,6 +244,12 @@
   </si>
   <si>
     <t>placeHolder</t>
+  </si>
+  <si>
+    <t>api</t>
+  </si>
+  <si>
+    <t>http://localhost:9001/tableData</t>
   </si>
 </sst>
 </file>
@@ -566,7 +560,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -577,7 +571,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -966,23 +960,18 @@
         <v>62</v>
       </c>
       <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
         <v>63</v>
       </c>
-      <c r="F12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G12" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="J12" t="b">
+      <c r="H12" s="1" t="b">
         <v>1</v>
       </c>
+      <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
@@ -992,7 +981,7 @@
         <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E13" t="s">
         <v>18</v>
@@ -1015,19 +1004,19 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C14" t="s">
         <v>46</v>
       </c>
       <c r="D14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E14" t="s">
         <v>18</v>
       </c>
       <c r="F14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
         <v>38</v>
@@ -1036,27 +1025,27 @@
         <v>1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G15" t="s">
         <v>38</v>
@@ -1065,10 +1054,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>